<commit_message>
update blog + update lapran tahfidz
</commit_message>
<xml_diff>
--- a/pesantren/tahfidz/laporan tahfidz/2023/11. november.xlsx
+++ b/pesantren/tahfidz/laporan tahfidz/2023/11. november.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ZEN-PROJECT\zen\pesantren\tahfidz\laporan tahfidz\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31689EF-6723-4B7D-A2BB-9AD8042AB2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB1CA73-8AC2-4059-BB0E-E946B73004DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="84">
   <si>
     <t>Keterangan</t>
   </si>
@@ -155,6 +155,129 @@
   </si>
   <si>
     <t>(Di juz 11, sampai 3A)</t>
+  </si>
+  <si>
+    <t>Persiapan Juziyah 2 (Juziyah tanggal 23)</t>
+  </si>
+  <si>
+    <t>5 juz</t>
+  </si>
+  <si>
+    <t>(Di juz 2, sampai 3A)</t>
+  </si>
+  <si>
+    <t>Persiapan Juziyah 1 (Juziyah tanggal 6) - Orangnya sakit</t>
+  </si>
+  <si>
+    <t>10 juz</t>
+  </si>
+  <si>
+    <t>Persiapan Syahadah (udah siap juz 5, 6, 7, dan 9) Syahadah pertengahan Desember</t>
+  </si>
+  <si>
+    <t>9 juz (juz 8 kurang lancar)</t>
+  </si>
+  <si>
+    <t>Radja</t>
+  </si>
+  <si>
+    <t>Faiq</t>
+  </si>
+  <si>
+    <t>Shinra</t>
+  </si>
+  <si>
+    <t>Idris</t>
+  </si>
+  <si>
+    <t>Fahri</t>
+  </si>
+  <si>
+    <t>Syahid</t>
+  </si>
+  <si>
+    <t>Kamil</t>
+  </si>
+  <si>
+    <t>Juz 4, 6A</t>
+  </si>
+  <si>
+    <t>5 halaman</t>
+  </si>
+  <si>
+    <t>4 juz (kurang juz 3)</t>
+  </si>
+  <si>
+    <t>(Di juz 3, sampai 4B)</t>
+  </si>
+  <si>
+    <t>Persiapan Syahadah (udah siap juz 5, 6, 7, dan 8) Syahadah akhir Desember</t>
+  </si>
+  <si>
+    <t>9 juz (juz 9 kurang setengah)</t>
+  </si>
+  <si>
+    <t>Persiapan Juziyah 5 (Juziyah tanggal 18)</t>
+  </si>
+  <si>
+    <t>5 juz (juz 2 dikit lagi)</t>
+  </si>
+  <si>
+    <t>(Di juz 5, sampai 2A)</t>
+  </si>
+  <si>
+    <t>Juz 1, 9A</t>
+  </si>
+  <si>
+    <t>5 kali</t>
+  </si>
+  <si>
+    <t>8 halaman</t>
+  </si>
+  <si>
+    <t>6 kali</t>
+  </si>
+  <si>
+    <t>2 juz</t>
+  </si>
+  <si>
+    <t>Juz 29, 1A</t>
+  </si>
+  <si>
+    <t>7 halaman</t>
+  </si>
+  <si>
+    <t>20 halaman</t>
+  </si>
+  <si>
+    <t>Persiapan Juziyah 1 (Juziyah tanggal 13)</t>
+  </si>
+  <si>
+    <t>Juz 29, 7B</t>
+  </si>
+  <si>
+    <t>14 halaman</t>
+  </si>
+  <si>
+    <t>Juz 29, 5A</t>
+  </si>
+  <si>
+    <t>12 halaman</t>
+  </si>
+  <si>
+    <t>3 kali (juz 8), 3 kali (juz 7)</t>
+  </si>
+  <si>
+    <t>Juz 29, 9A</t>
+  </si>
+  <si>
+    <t>13 halaman</t>
+  </si>
+  <si>
+    <t>Juz 30, 8A</t>
+  </si>
+  <si>
+    <t>1 juz</t>
   </si>
 </sst>
 </file>
@@ -665,10 +788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC927C4-ECEF-462E-B302-B5C83C575FD9}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +800,7 @@
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="73.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -712,7 +835,7 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -723,13 +846,10 @@
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -740,13 +860,13 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -774,10 +894,10 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -785,16 +905,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -804,8 +924,11 @@
       <c r="B8" t="s">
         <v>14</v>
       </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
         <v>36</v>
@@ -819,10 +942,10 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -833,13 +956,135 @@
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>